<commit_message>
input satu data hasil prediksi pake tabel
</commit_message>
<xml_diff>
--- a/downloads/jan-apr2024_-_Copy.xlsx
+++ b/downloads/jan-apr2024_-_Copy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Nh Label</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Prediksi Suhu</t>
         </is>
       </c>
@@ -452,7 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29.7118424</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>29.7065722</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>29.7118424</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>29.7065722</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29.7118424</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>29.7065722</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29.71184047</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>29.70656551</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29.71184625</v>
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>29.70658557</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>29.71183084</v>
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>29.70653207</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>29.7118424</v>
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>29.7065722</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +548,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>29.7118424</v>
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>29.7065722</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>29.7118424</v>
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>29.7065722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>